<commit_message>
Inserindo dados na lista
</commit_message>
<xml_diff>
--- a/app/data/db_calc_perfumaria.xlsx
+++ b/app/data/db_calc_perfumaria.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>4000.0</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>4000.0</t>
         </is>
       </c>
     </row>

</xml_diff>